<commit_message>
finish v2 csv import in task_1d, minor improvements
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_e.xlsx
+++ b/data/fabian/output/processed_e.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
finish v2 csv import in task_1e
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_e.xlsx
+++ b/data/fabian/output/processed_e.xlsx
@@ -558,7 +558,7 @@
         <v>-49.05333333333333</v>
       </c>
       <c r="I2" t="n">
-        <v>-12.002</v>
+        <v>-12.00333333333333</v>
       </c>
       <c r="J2" t="n">
         <v>19.93666666666667</v>
@@ -579,7 +579,7 @@
         <v>9.063333333333334</v>
       </c>
       <c r="P2" t="n">
-        <v>180.6333333333333</v>
+        <v>180.6266666666667</v>
       </c>
       <c r="Q2" t="n">
         <v>5.62</v>
@@ -619,7 +619,7 @@
         <v>-49.05333333333333</v>
       </c>
       <c r="I3" t="n">
-        <v>-12.002</v>
+        <v>-12.00333333333333</v>
       </c>
       <c r="J3" t="n">
         <v>19.93666666666667</v>
@@ -640,7 +640,7 @@
         <v>9.063333333333334</v>
       </c>
       <c r="P3" t="n">
-        <v>180.6333333333333</v>
+        <v>180.6266666666667</v>
       </c>
       <c r="Q3" t="n">
         <v>5.62</v>
@@ -662,7 +662,7 @@
         <v>-94.48666666666668</v>
       </c>
       <c r="C4" t="n">
-        <v>18.12166666666667</v>
+        <v>18.12333333333333</v>
       </c>
       <c r="D4" t="n">
         <v>30.00666666666667</v>
@@ -680,7 +680,7 @@
         <v>-62.08333333333334</v>
       </c>
       <c r="I4" t="n">
-        <v>-11.99933333333333</v>
+        <v>-12</v>
       </c>
       <c r="J4" t="n">
         <v>19.87</v>
@@ -701,7 +701,7 @@
         <v>9.060000000000002</v>
       </c>
       <c r="P4" t="n">
-        <v>180.0666666666667</v>
+        <v>180.05</v>
       </c>
       <c r="Q4" t="n">
         <v>5.62</v>
@@ -723,7 +723,7 @@
         <v>-94.62333333333333</v>
       </c>
       <c r="C5" t="n">
-        <v>18.11933333333333</v>
+        <v>18.12</v>
       </c>
       <c r="D5" t="n">
         <v>30.00666666666666</v>
@@ -759,10 +759,10 @@
         <v>-47.31333333333333</v>
       </c>
       <c r="O5" t="n">
-        <v>9.070000000000002</v>
+        <v>9.063333333333333</v>
       </c>
       <c r="P5" t="n">
-        <v>180.0666666666667</v>
+        <v>180.0533333333333</v>
       </c>
       <c r="Q5" t="n">
         <v>5.62</v>
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-93.95333333333333</v>
+        <v>-93.96333333333332</v>
       </c>
       <c r="C6" t="n">
         <v>18.12</v>
@@ -802,7 +802,7 @@
         <v>-62.89333333333334</v>
       </c>
       <c r="I6" t="n">
-        <v>-12.002</v>
+        <v>-12.00333333333333</v>
       </c>
       <c r="J6" t="n">
         <v>20.18</v>
@@ -817,13 +817,13 @@
         <v>1.22</v>
       </c>
       <c r="N6" t="n">
-        <v>-46.98266666666666</v>
+        <v>-46.98333333333333</v>
       </c>
       <c r="O6" t="n">
-        <v>9.090666666666664</v>
+        <v>9.060000000000002</v>
       </c>
       <c r="P6" t="n">
-        <v>182.8</v>
+        <v>182.8066666666666</v>
       </c>
       <c r="Q6" t="n">
         <v>5.62</v>
@@ -842,10 +842,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-93.45666666666666</v>
+        <v>-93.46333333333332</v>
       </c>
       <c r="C7" t="n">
-        <v>18.12233333333333</v>
+        <v>18.12333333333333</v>
       </c>
       <c r="D7" t="n">
         <v>53.25</v>
@@ -863,7 +863,7 @@
         <v>-62.59</v>
       </c>
       <c r="I7" t="n">
-        <v>-11.99866666666667</v>
+        <v>-12</v>
       </c>
       <c r="J7" t="n">
         <v>35.26666666666667</v>
@@ -878,13 +878,13 @@
         <v>1.16</v>
       </c>
       <c r="N7" t="n">
-        <v>-46.72933333333333</v>
+        <v>-46.73</v>
       </c>
       <c r="O7" t="n">
-        <v>9.059666666666667</v>
+        <v>9.06</v>
       </c>
       <c r="P7" t="n">
-        <v>319.5</v>
+        <v>319.51</v>
       </c>
       <c r="Q7" t="n">
         <v>5.62</v>
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-93.45666666666666</v>
+        <v>-93.46333333333332</v>
       </c>
       <c r="C8" t="n">
-        <v>18.12233333333333</v>
+        <v>18.12333333333333</v>
       </c>
       <c r="D8" t="n">
         <v>53.25</v>
@@ -924,7 +924,7 @@
         <v>-62.59</v>
       </c>
       <c r="I8" t="n">
-        <v>-11.99866666666667</v>
+        <v>-12</v>
       </c>
       <c r="J8" t="n">
         <v>35.26666666666667</v>
@@ -939,13 +939,13 @@
         <v>1.16</v>
       </c>
       <c r="N8" t="n">
-        <v>-46.72933333333333</v>
+        <v>-46.73</v>
       </c>
       <c r="O8" t="n">
-        <v>9.059666666666667</v>
+        <v>9.059999999999997</v>
       </c>
       <c r="P8" t="n">
-        <v>319.5</v>
+        <v>319.51</v>
       </c>
       <c r="Q8" t="n">
         <v>5.62</v>
@@ -964,7 +964,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-93.95333333333333</v>
+        <v>-93.96333333333332</v>
       </c>
       <c r="C9" t="n">
         <v>18.12</v>
@@ -985,7 +985,7 @@
         <v>-62.89333333333334</v>
       </c>
       <c r="I9" t="n">
-        <v>-12.002</v>
+        <v>-12.00333333333333</v>
       </c>
       <c r="J9" t="n">
         <v>20.18</v>
@@ -1000,13 +1000,13 @@
         <v>1.22</v>
       </c>
       <c r="N9" t="n">
-        <v>-46.98266666666667</v>
+        <v>-46.98333333333333</v>
       </c>
       <c r="O9" t="n">
-        <v>9.090666666666664</v>
+        <v>9.060000000000002</v>
       </c>
       <c r="P9" t="n">
-        <v>182.8</v>
+        <v>182.8066666666666</v>
       </c>
       <c r="Q9" t="n">
         <v>5.62</v>
@@ -1028,7 +1028,7 @@
         <v>-94.62333333333333</v>
       </c>
       <c r="C10" t="n">
-        <v>18.11933333333333</v>
+        <v>18.12</v>
       </c>
       <c r="D10" t="n">
         <v>30.00666666666666</v>
@@ -1064,10 +1064,10 @@
         <v>-47.31333333333333</v>
       </c>
       <c r="O10" t="n">
-        <v>9.070000000000002</v>
+        <v>9.063333333333333</v>
       </c>
       <c r="P10" t="n">
-        <v>180.0666666666667</v>
+        <v>180.0533333333333</v>
       </c>
       <c r="Q10" t="n">
         <v>5.62</v>
@@ -1089,7 +1089,7 @@
         <v>-94.48666666666668</v>
       </c>
       <c r="C11" t="n">
-        <v>18.12166666666667</v>
+        <v>18.12333333333333</v>
       </c>
       <c r="D11" t="n">
         <v>30.00666666666667</v>
@@ -1107,7 +1107,7 @@
         <v>-62.08333333333334</v>
       </c>
       <c r="I11" t="n">
-        <v>-11.99933333333333</v>
+        <v>-12</v>
       </c>
       <c r="J11" t="n">
         <v>19.87</v>
@@ -1128,7 +1128,7 @@
         <v>9.060000000000002</v>
       </c>
       <c r="P11" t="n">
-        <v>180.0666666666667</v>
+        <v>180.05</v>
       </c>
       <c r="Q11" t="n">
         <v>5.62</v>

</xml_diff>

<commit_message>
round the sigmaXX, sigmaYY, sigmaXY values to 2 decimal places
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_e.xlsx
+++ b/data/fabian/output/processed_e.xlsx
@@ -537,13 +537,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-72.42333333333333</v>
+        <v>-72.42</v>
       </c>
       <c r="C2" t="n">
         <v>18.12</v>
       </c>
       <c r="D2" t="n">
-        <v>30.10666666666667</v>
+        <v>30.11</v>
       </c>
       <c r="E2" t="n">
         <v>5.62</v>
@@ -555,13 +555,13 @@
         <v>1.57</v>
       </c>
       <c r="H2" t="n">
-        <v>-49.05333333333333</v>
+        <v>-49.05</v>
       </c>
       <c r="I2" t="n">
-        <v>-12.00333333333333</v>
+        <v>-12</v>
       </c>
       <c r="J2" t="n">
-        <v>19.93666666666667</v>
+        <v>19.94</v>
       </c>
       <c r="K2" t="n">
         <v>5.62</v>
@@ -576,10 +576,10 @@
         <v>-36.21</v>
       </c>
       <c r="O2" t="n">
-        <v>9.063333333333334</v>
+        <v>9.06</v>
       </c>
       <c r="P2" t="n">
-        <v>180.6266666666667</v>
+        <v>180.63</v>
       </c>
       <c r="Q2" t="n">
         <v>5.62</v>
@@ -598,13 +598,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-72.42333333333333</v>
+        <v>-72.42</v>
       </c>
       <c r="C3" t="n">
         <v>18.12</v>
       </c>
       <c r="D3" t="n">
-        <v>30.10666666666667</v>
+        <v>30.11</v>
       </c>
       <c r="E3" t="n">
         <v>5.62</v>
@@ -616,13 +616,13 @@
         <v>1.57</v>
       </c>
       <c r="H3" t="n">
-        <v>-49.05333333333333</v>
+        <v>-49.05</v>
       </c>
       <c r="I3" t="n">
-        <v>-12.00333333333333</v>
+        <v>-12</v>
       </c>
       <c r="J3" t="n">
-        <v>19.93666666666667</v>
+        <v>19.94</v>
       </c>
       <c r="K3" t="n">
         <v>5.62</v>
@@ -637,10 +637,10 @@
         <v>-36.21</v>
       </c>
       <c r="O3" t="n">
-        <v>9.063333333333334</v>
+        <v>9.06</v>
       </c>
       <c r="P3" t="n">
-        <v>180.6266666666667</v>
+        <v>180.63</v>
       </c>
       <c r="Q3" t="n">
         <v>5.62</v>
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-94.48666666666668</v>
+        <v>-94.48999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>18.12333333333333</v>
+        <v>18.12</v>
       </c>
       <c r="D4" t="n">
-        <v>30.00666666666667</v>
+        <v>30.01</v>
       </c>
       <c r="E4" t="n">
         <v>5.62</v>
@@ -677,7 +677,7 @@
         <v>1.17</v>
       </c>
       <c r="H4" t="n">
-        <v>-62.08333333333334</v>
+        <v>-62.08</v>
       </c>
       <c r="I4" t="n">
         <v>-12</v>
@@ -695,10 +695,10 @@
         <v>1.24</v>
       </c>
       <c r="N4" t="n">
-        <v>-47.24333333333334</v>
+        <v>-47.24</v>
       </c>
       <c r="O4" t="n">
-        <v>9.060000000000002</v>
+        <v>9.06</v>
       </c>
       <c r="P4" t="n">
         <v>180.05</v>
@@ -720,13 +720,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-94.62333333333333</v>
+        <v>-94.62</v>
       </c>
       <c r="C5" t="n">
         <v>18.12</v>
       </c>
       <c r="D5" t="n">
-        <v>30.00666666666666</v>
+        <v>30.01</v>
       </c>
       <c r="E5" t="n">
         <v>5.62</v>
@@ -738,13 +738,13 @@
         <v>1.17</v>
       </c>
       <c r="H5" t="n">
-        <v>-63.01666666666667</v>
+        <v>-63.02</v>
       </c>
       <c r="I5" t="n">
         <v>-12</v>
       </c>
       <c r="J5" t="n">
-        <v>19.87333333333333</v>
+        <v>19.87</v>
       </c>
       <c r="K5" t="n">
         <v>5.62</v>
@@ -756,13 +756,13 @@
         <v>1.22</v>
       </c>
       <c r="N5" t="n">
-        <v>-47.31333333333333</v>
+        <v>-47.31</v>
       </c>
       <c r="O5" t="n">
-        <v>9.063333333333333</v>
+        <v>9.06</v>
       </c>
       <c r="P5" t="n">
-        <v>180.0533333333333</v>
+        <v>180.05</v>
       </c>
       <c r="Q5" t="n">
         <v>5.62</v>
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-93.96333333333332</v>
+        <v>-93.95999999999999</v>
       </c>
       <c r="C6" t="n">
         <v>18.12</v>
@@ -799,10 +799,10 @@
         <v>1.18</v>
       </c>
       <c r="H6" t="n">
-        <v>-62.89333333333334</v>
+        <v>-62.89</v>
       </c>
       <c r="I6" t="n">
-        <v>-12.00333333333333</v>
+        <v>-12</v>
       </c>
       <c r="J6" t="n">
         <v>20.18</v>
@@ -817,13 +817,13 @@
         <v>1.22</v>
       </c>
       <c r="N6" t="n">
-        <v>-46.98333333333333</v>
+        <v>-46.98</v>
       </c>
       <c r="O6" t="n">
-        <v>9.060000000000002</v>
+        <v>9.06</v>
       </c>
       <c r="P6" t="n">
-        <v>182.8066666666666</v>
+        <v>182.81</v>
       </c>
       <c r="Q6" t="n">
         <v>5.62</v>
@@ -842,10 +842,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-93.46333333333332</v>
+        <v>-93.45999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>18.12333333333333</v>
+        <v>18.12</v>
       </c>
       <c r="D7" t="n">
         <v>53.25</v>
@@ -866,7 +866,7 @@
         <v>-12</v>
       </c>
       <c r="J7" t="n">
-        <v>35.26666666666667</v>
+        <v>35.27</v>
       </c>
       <c r="K7" t="n">
         <v>5.62</v>
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-93.46333333333332</v>
+        <v>-93.45999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>18.12333333333333</v>
+        <v>18.12</v>
       </c>
       <c r="D8" t="n">
         <v>53.25</v>
@@ -927,7 +927,7 @@
         <v>-12</v>
       </c>
       <c r="J8" t="n">
-        <v>35.26666666666667</v>
+        <v>35.27</v>
       </c>
       <c r="K8" t="n">
         <v>5.62</v>
@@ -942,7 +942,7 @@
         <v>-46.73</v>
       </c>
       <c r="O8" t="n">
-        <v>9.059999999999997</v>
+        <v>9.06</v>
       </c>
       <c r="P8" t="n">
         <v>319.51</v>
@@ -964,7 +964,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-93.96333333333332</v>
+        <v>-93.95999999999999</v>
       </c>
       <c r="C9" t="n">
         <v>18.12</v>
@@ -982,10 +982,10 @@
         <v>1.18</v>
       </c>
       <c r="H9" t="n">
-        <v>-62.89333333333334</v>
+        <v>-62.89</v>
       </c>
       <c r="I9" t="n">
-        <v>-12.00333333333333</v>
+        <v>-12</v>
       </c>
       <c r="J9" t="n">
         <v>20.18</v>
@@ -1000,13 +1000,13 @@
         <v>1.22</v>
       </c>
       <c r="N9" t="n">
-        <v>-46.98333333333333</v>
+        <v>-46.98</v>
       </c>
       <c r="O9" t="n">
-        <v>9.060000000000002</v>
+        <v>9.06</v>
       </c>
       <c r="P9" t="n">
-        <v>182.8066666666666</v>
+        <v>182.81</v>
       </c>
       <c r="Q9" t="n">
         <v>5.62</v>
@@ -1025,13 +1025,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-94.62333333333333</v>
+        <v>-94.62</v>
       </c>
       <c r="C10" t="n">
         <v>18.12</v>
       </c>
       <c r="D10" t="n">
-        <v>30.00666666666666</v>
+        <v>30.01</v>
       </c>
       <c r="E10" t="n">
         <v>5.62</v>
@@ -1043,13 +1043,13 @@
         <v>1.17</v>
       </c>
       <c r="H10" t="n">
-        <v>-63.01666666666667</v>
+        <v>-63.02</v>
       </c>
       <c r="I10" t="n">
         <v>-12</v>
       </c>
       <c r="J10" t="n">
-        <v>19.87333333333333</v>
+        <v>19.87</v>
       </c>
       <c r="K10" t="n">
         <v>5.62</v>
@@ -1061,13 +1061,13 @@
         <v>1.22</v>
       </c>
       <c r="N10" t="n">
-        <v>-47.31333333333333</v>
+        <v>-47.31</v>
       </c>
       <c r="O10" t="n">
-        <v>9.063333333333333</v>
+        <v>9.06</v>
       </c>
       <c r="P10" t="n">
-        <v>180.0533333333333</v>
+        <v>180.05</v>
       </c>
       <c r="Q10" t="n">
         <v>5.62</v>
@@ -1086,13 +1086,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-94.48666666666668</v>
+        <v>-94.48999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>18.12333333333333</v>
+        <v>18.12</v>
       </c>
       <c r="D11" t="n">
-        <v>30.00666666666667</v>
+        <v>30.01</v>
       </c>
       <c r="E11" t="n">
         <v>5.62</v>
@@ -1104,7 +1104,7 @@
         <v>1.17</v>
       </c>
       <c r="H11" t="n">
-        <v>-62.08333333333334</v>
+        <v>-62.08</v>
       </c>
       <c r="I11" t="n">
         <v>-12</v>
@@ -1122,10 +1122,10 @@
         <v>1.24</v>
       </c>
       <c r="N11" t="n">
-        <v>-47.24333333333334</v>
+        <v>-47.24</v>
       </c>
       <c r="O11" t="n">
-        <v>9.060000000000002</v>
+        <v>9.06</v>
       </c>
       <c r="P11" t="n">
         <v>180.05</v>

</xml_diff>

<commit_message>
add rounding to task_1e
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_e.xlsx
+++ b/data/fabian/output/processed_e.xlsx
@@ -692,7 +692,7 @@
         <v>3.23</v>
       </c>
       <c r="M4" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="N4" t="n">
         <v>-47.24</v>
@@ -1119,7 +1119,7 @@
         <v>3.23</v>
       </c>
       <c r="M11" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="N11" t="n">
         <v>-47.24</v>

</xml_diff>

<commit_message>
for panels.py add 1.5 for ultimate loads
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_e.xlsx
+++ b/data/fabian/output/processed_e.xlsx
@@ -552,7 +552,7 @@
         <v>5.05</v>
       </c>
       <c r="G2" t="n">
-        <v>1.57</v>
+        <v>1.01</v>
       </c>
       <c r="H2" t="n">
         <v>-49.05</v>
@@ -570,7 +570,7 @@
         <v>3.04</v>
       </c>
       <c r="M2" t="n">
-        <v>1.46</v>
+        <v>0.96</v>
       </c>
       <c r="N2" t="n">
         <v>-36.21</v>
@@ -588,7 +588,7 @@
         <v>5.05</v>
       </c>
       <c r="S2" t="n">
-        <v>0.49</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="3">
@@ -613,7 +613,7 @@
         <v>5.05</v>
       </c>
       <c r="G3" t="n">
-        <v>1.57</v>
+        <v>1.01</v>
       </c>
       <c r="H3" t="n">
         <v>-49.05</v>
@@ -631,7 +631,7 @@
         <v>3.04</v>
       </c>
       <c r="M3" t="n">
-        <v>1.46</v>
+        <v>0.96</v>
       </c>
       <c r="N3" t="n">
         <v>-36.21</v>
@@ -649,7 +649,7 @@
         <v>5.05</v>
       </c>
       <c r="S3" t="n">
-        <v>0.49</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="4">
@@ -674,7 +674,7 @@
         <v>4.83</v>
       </c>
       <c r="G4" t="n">
-        <v>1.17</v>
+        <v>0.76</v>
       </c>
       <c r="H4" t="n">
         <v>-62.08</v>
@@ -692,7 +692,7 @@
         <v>3.23</v>
       </c>
       <c r="M4" t="n">
-        <v>1.23</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="N4" t="n">
         <v>-47.24</v>
@@ -710,7 +710,7 @@
         <v>4.83</v>
       </c>
       <c r="S4" t="n">
-        <v>0.47</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="5">
@@ -735,7 +735,7 @@
         <v>4.83</v>
       </c>
       <c r="G5" t="n">
-        <v>1.17</v>
+        <v>0.76</v>
       </c>
       <c r="H5" t="n">
         <v>-63.02</v>
@@ -753,7 +753,7 @@
         <v>3.24</v>
       </c>
       <c r="M5" t="n">
-        <v>1.22</v>
+        <v>0.8</v>
       </c>
       <c r="N5" t="n">
         <v>-47.31</v>
@@ -771,7 +771,7 @@
         <v>4.83</v>
       </c>
       <c r="S5" t="n">
-        <v>0.47</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="6">
@@ -796,7 +796,7 @@
         <v>4.84</v>
       </c>
       <c r="G6" t="n">
-        <v>1.18</v>
+        <v>0.76</v>
       </c>
       <c r="H6" t="n">
         <v>-62.89</v>
@@ -814,7 +814,7 @@
         <v>3.24</v>
       </c>
       <c r="M6" t="n">
-        <v>1.22</v>
+        <v>0.8</v>
       </c>
       <c r="N6" t="n">
         <v>-46.98</v>
@@ -832,7 +832,7 @@
         <v>4.84</v>
       </c>
       <c r="S6" t="n">
-        <v>0.46</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="7">
@@ -857,7 +857,7 @@
         <v>4.84</v>
       </c>
       <c r="G7" t="n">
-        <v>1.06</v>
+        <v>0.65</v>
       </c>
       <c r="H7" t="n">
         <v>-62.59</v>
@@ -875,7 +875,7 @@
         <v>3.23</v>
       </c>
       <c r="M7" t="n">
-        <v>1.16</v>
+        <v>0.74</v>
       </c>
       <c r="N7" t="n">
         <v>-46.73</v>
@@ -893,7 +893,7 @@
         <v>4.84</v>
       </c>
       <c r="S7" t="n">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="8">
@@ -918,7 +918,7 @@
         <v>4.84</v>
       </c>
       <c r="G8" t="n">
-        <v>1.06</v>
+        <v>0.65</v>
       </c>
       <c r="H8" t="n">
         <v>-62.59</v>
@@ -936,7 +936,7 @@
         <v>3.23</v>
       </c>
       <c r="M8" t="n">
-        <v>1.16</v>
+        <v>0.74</v>
       </c>
       <c r="N8" t="n">
         <v>-46.73</v>
@@ -954,7 +954,7 @@
         <v>4.84</v>
       </c>
       <c r="S8" t="n">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="9">
@@ -979,7 +979,7 @@
         <v>4.84</v>
       </c>
       <c r="G9" t="n">
-        <v>1.18</v>
+        <v>0.76</v>
       </c>
       <c r="H9" t="n">
         <v>-62.89</v>
@@ -997,7 +997,7 @@
         <v>3.24</v>
       </c>
       <c r="M9" t="n">
-        <v>1.22</v>
+        <v>0.8</v>
       </c>
       <c r="N9" t="n">
         <v>-46.98</v>
@@ -1015,7 +1015,7 @@
         <v>4.84</v>
       </c>
       <c r="S9" t="n">
-        <v>0.46</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="10">
@@ -1040,7 +1040,7 @@
         <v>4.83</v>
       </c>
       <c r="G10" t="n">
-        <v>1.17</v>
+        <v>0.76</v>
       </c>
       <c r="H10" t="n">
         <v>-63.02</v>
@@ -1058,7 +1058,7 @@
         <v>3.24</v>
       </c>
       <c r="M10" t="n">
-        <v>1.22</v>
+        <v>0.8</v>
       </c>
       <c r="N10" t="n">
         <v>-47.31</v>
@@ -1076,7 +1076,7 @@
         <v>4.83</v>
       </c>
       <c r="S10" t="n">
-        <v>0.47</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="11">
@@ -1101,7 +1101,7 @@
         <v>4.83</v>
       </c>
       <c r="G11" t="n">
-        <v>1.17</v>
+        <v>0.76</v>
       </c>
       <c r="H11" t="n">
         <v>-62.08</v>
@@ -1119,7 +1119,7 @@
         <v>3.23</v>
       </c>
       <c r="M11" t="n">
-        <v>1.23</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="N11" t="n">
         <v>-47.24</v>
@@ -1137,7 +1137,7 @@
         <v>4.83</v>
       </c>
       <c r="S11" t="n">
-        <v>0.47</v>
+        <v>0.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update my data only
</commit_message>
<xml_diff>
--- a/data/fabian/output/processed_e.xlsx
+++ b/data/fabian/output/processed_e.xlsx
@@ -537,58 +537,58 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-72.42</v>
+        <v>-72.419</v>
       </c>
       <c r="C2" t="n">
         <v>18.12</v>
       </c>
       <c r="D2" t="n">
-        <v>30.11</v>
+        <v>30.104</v>
       </c>
       <c r="E2" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F2" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="G2" t="n">
-        <v>1.01</v>
+        <v>1.008</v>
       </c>
       <c r="H2" t="n">
-        <v>-49.05</v>
+        <v>-74.071</v>
       </c>
       <c r="I2" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J2" t="n">
-        <v>19.94</v>
+        <v>30.104</v>
       </c>
       <c r="K2" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L2" t="n">
         <v>3.04</v>
       </c>
       <c r="M2" t="n">
-        <v>0.96</v>
+        <v>0.621</v>
       </c>
       <c r="N2" t="n">
-        <v>-36.21</v>
+        <v>-23.98</v>
       </c>
       <c r="O2" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P2" t="n">
-        <v>180.63</v>
+        <v>119.619</v>
       </c>
       <c r="Q2" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R2" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="S2" t="n">
-        <v>0.23</v>
+        <v>0.497</v>
       </c>
     </row>
     <row r="3">
@@ -598,58 +598,58 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-72.42</v>
+        <v>-72.419</v>
       </c>
       <c r="C3" t="n">
         <v>18.12</v>
       </c>
       <c r="D3" t="n">
-        <v>30.11</v>
+        <v>30.104</v>
       </c>
       <c r="E3" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F3" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="G3" t="n">
-        <v>1.01</v>
+        <v>1.008</v>
       </c>
       <c r="H3" t="n">
-        <v>-49.05</v>
+        <v>-74.071</v>
       </c>
       <c r="I3" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J3" t="n">
-        <v>19.94</v>
+        <v>30.104</v>
       </c>
       <c r="K3" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L3" t="n">
         <v>3.04</v>
       </c>
       <c r="M3" t="n">
-        <v>0.96</v>
+        <v>0.621</v>
       </c>
       <c r="N3" t="n">
-        <v>-36.21</v>
+        <v>-23.98</v>
       </c>
       <c r="O3" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P3" t="n">
-        <v>180.63</v>
+        <v>119.619</v>
       </c>
       <c r="Q3" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R3" t="n">
-        <v>5.05</v>
+        <v>5.051</v>
       </c>
       <c r="S3" t="n">
-        <v>0.23</v>
+        <v>0.497</v>
       </c>
     </row>
     <row r="4">
@@ -659,58 +659,58 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-94.48999999999999</v>
+        <v>-94.486</v>
       </c>
       <c r="C4" t="n">
         <v>18.12</v>
       </c>
       <c r="D4" t="n">
-        <v>30.01</v>
+        <v>30.008</v>
       </c>
       <c r="E4" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F4" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="G4" t="n">
-        <v>0.76</v>
+        <v>0.761</v>
       </c>
       <c r="H4" t="n">
-        <v>-62.08</v>
+        <v>-93.742</v>
       </c>
       <c r="I4" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J4" t="n">
-        <v>19.87</v>
+        <v>30.008</v>
       </c>
       <c r="K4" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L4" t="n">
-        <v>3.23</v>
+        <v>3.228</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.527</v>
       </c>
       <c r="N4" t="n">
-        <v>-47.24</v>
+        <v>-31.287</v>
       </c>
       <c r="O4" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P4" t="n">
-        <v>180.05</v>
+        <v>119.237</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R4" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="S4" t="n">
-        <v>0.22</v>
+        <v>0.475</v>
       </c>
     </row>
     <row r="5">
@@ -720,16 +720,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-94.62</v>
+        <v>-94.624</v>
       </c>
       <c r="C5" t="n">
         <v>18.12</v>
       </c>
       <c r="D5" t="n">
-        <v>30.01</v>
+        <v>30.009</v>
       </c>
       <c r="E5" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F5" t="n">
         <v>4.83</v>
@@ -738,40 +738,40 @@
         <v>0.76</v>
       </c>
       <c r="H5" t="n">
-        <v>-63.02</v>
+        <v>-95.157</v>
       </c>
       <c r="I5" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J5" t="n">
-        <v>19.87</v>
+        <v>30.009</v>
       </c>
       <c r="K5" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L5" t="n">
-        <v>3.24</v>
+        <v>3.239</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8</v>
+        <v>0.521</v>
       </c>
       <c r="N5" t="n">
-        <v>-47.31</v>
+        <v>-31.333</v>
       </c>
       <c r="O5" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P5" t="n">
-        <v>180.05</v>
+        <v>119.241</v>
       </c>
       <c r="Q5" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R5" t="n">
         <v>4.83</v>
       </c>
       <c r="S5" t="n">
-        <v>0.22</v>
+        <v>0.474</v>
       </c>
     </row>
     <row r="6">
@@ -781,58 +781,58 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-93.95999999999999</v>
+        <v>-93.96299999999999</v>
       </c>
       <c r="C6" t="n">
         <v>18.12</v>
       </c>
       <c r="D6" t="n">
-        <v>30.47</v>
+        <v>30.468</v>
       </c>
       <c r="E6" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F6" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="G6" t="n">
-        <v>0.76</v>
+        <v>0.764</v>
       </c>
       <c r="H6" t="n">
-        <v>-62.89</v>
+        <v>-94.96599999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J6" t="n">
-        <v>20.18</v>
+        <v>30.468</v>
       </c>
       <c r="K6" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L6" t="n">
-        <v>3.24</v>
+        <v>3.237</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8</v>
+        <v>0.521</v>
       </c>
       <c r="N6" t="n">
-        <v>-46.98</v>
+        <v>-31.113</v>
       </c>
       <c r="O6" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P6" t="n">
-        <v>182.81</v>
+        <v>121.064</v>
       </c>
       <c r="Q6" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R6" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="S6" t="n">
-        <v>0.22</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="7">
@@ -842,58 +842,58 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-93.45999999999999</v>
+        <v>-93.462</v>
       </c>
       <c r="C7" t="n">
         <v>18.12</v>
       </c>
       <c r="D7" t="n">
-        <v>53.25</v>
+        <v>53.252</v>
       </c>
       <c r="E7" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F7" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="G7" t="n">
-        <v>0.65</v>
+        <v>0.653</v>
       </c>
       <c r="H7" t="n">
-        <v>-62.59</v>
+        <v>-94.509</v>
       </c>
       <c r="I7" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J7" t="n">
-        <v>35.27</v>
+        <v>53.252</v>
       </c>
       <c r="K7" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L7" t="n">
-        <v>3.23</v>
+        <v>3.234</v>
       </c>
       <c r="M7" t="n">
-        <v>0.74</v>
+        <v>0.467</v>
       </c>
       <c r="N7" t="n">
-        <v>-46.73</v>
+        <v>-30.948</v>
       </c>
       <c r="O7" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P7" t="n">
-        <v>319.51</v>
+        <v>211.597</v>
       </c>
       <c r="Q7" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R7" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="S7" t="n">
-        <v>0.08</v>
+        <v>0.173</v>
       </c>
     </row>
     <row r="8">
@@ -903,58 +903,58 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-93.45999999999999</v>
+        <v>-93.462</v>
       </c>
       <c r="C8" t="n">
         <v>18.12</v>
       </c>
       <c r="D8" t="n">
-        <v>53.25</v>
+        <v>53.252</v>
       </c>
       <c r="E8" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F8" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="G8" t="n">
-        <v>0.65</v>
+        <v>0.653</v>
       </c>
       <c r="H8" t="n">
-        <v>-62.59</v>
+        <v>-94.509</v>
       </c>
       <c r="I8" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J8" t="n">
-        <v>35.27</v>
+        <v>53.252</v>
       </c>
       <c r="K8" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L8" t="n">
-        <v>3.23</v>
+        <v>3.234</v>
       </c>
       <c r="M8" t="n">
-        <v>0.74</v>
+        <v>0.467</v>
       </c>
       <c r="N8" t="n">
-        <v>-46.73</v>
+        <v>-30.948</v>
       </c>
       <c r="O8" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P8" t="n">
-        <v>319.51</v>
+        <v>211.597</v>
       </c>
       <c r="Q8" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R8" t="n">
-        <v>4.84</v>
+        <v>4.842</v>
       </c>
       <c r="S8" t="n">
-        <v>0.08</v>
+        <v>0.173</v>
       </c>
     </row>
     <row r="9">
@@ -964,58 +964,58 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-93.95999999999999</v>
+        <v>-93.96299999999999</v>
       </c>
       <c r="C9" t="n">
         <v>18.12</v>
       </c>
       <c r="D9" t="n">
-        <v>30.47</v>
+        <v>30.468</v>
       </c>
       <c r="E9" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F9" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="G9" t="n">
-        <v>0.76</v>
+        <v>0.764</v>
       </c>
       <c r="H9" t="n">
-        <v>-62.89</v>
+        <v>-94.96599999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J9" t="n">
-        <v>20.18</v>
+        <v>30.468</v>
       </c>
       <c r="K9" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L9" t="n">
-        <v>3.24</v>
+        <v>3.237</v>
       </c>
       <c r="M9" t="n">
-        <v>0.8</v>
+        <v>0.521</v>
       </c>
       <c r="N9" t="n">
-        <v>-46.98</v>
+        <v>-31.113</v>
       </c>
       <c r="O9" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P9" t="n">
-        <v>182.81</v>
+        <v>121.064</v>
       </c>
       <c r="Q9" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R9" t="n">
-        <v>4.84</v>
+        <v>4.836</v>
       </c>
       <c r="S9" t="n">
-        <v>0.22</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="10">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-94.62</v>
+        <v>-94.624</v>
       </c>
       <c r="C10" t="n">
         <v>18.12</v>
       </c>
       <c r="D10" t="n">
-        <v>30.01</v>
+        <v>30.009</v>
       </c>
       <c r="E10" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F10" t="n">
         <v>4.83</v>
@@ -1043,40 +1043,40 @@
         <v>0.76</v>
       </c>
       <c r="H10" t="n">
-        <v>-63.02</v>
+        <v>-95.157</v>
       </c>
       <c r="I10" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J10" t="n">
-        <v>19.87</v>
+        <v>30.009</v>
       </c>
       <c r="K10" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L10" t="n">
-        <v>3.24</v>
+        <v>3.239</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8</v>
+        <v>0.521</v>
       </c>
       <c r="N10" t="n">
-        <v>-47.31</v>
+        <v>-31.333</v>
       </c>
       <c r="O10" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P10" t="n">
-        <v>180.05</v>
+        <v>119.241</v>
       </c>
       <c r="Q10" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R10" t="n">
         <v>4.83</v>
       </c>
       <c r="S10" t="n">
-        <v>0.22</v>
+        <v>0.474</v>
       </c>
     </row>
     <row r="11">
@@ -1086,58 +1086,58 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-94.48999999999999</v>
+        <v>-94.486</v>
       </c>
       <c r="C11" t="n">
         <v>18.12</v>
       </c>
       <c r="D11" t="n">
-        <v>30.01</v>
+        <v>30.008</v>
       </c>
       <c r="E11" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="F11" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="G11" t="n">
-        <v>0.76</v>
+        <v>0.761</v>
       </c>
       <c r="H11" t="n">
-        <v>-62.08</v>
+        <v>-93.742</v>
       </c>
       <c r="I11" t="n">
-        <v>-12</v>
+        <v>-18.12</v>
       </c>
       <c r="J11" t="n">
-        <v>19.87</v>
+        <v>30.008</v>
       </c>
       <c r="K11" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="L11" t="n">
-        <v>3.23</v>
+        <v>3.228</v>
       </c>
       <c r="M11" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.527</v>
       </c>
       <c r="N11" t="n">
-        <v>-47.24</v>
+        <v>-31.287</v>
       </c>
       <c r="O11" t="n">
-        <v>9.06</v>
+        <v>6</v>
       </c>
       <c r="P11" t="n">
-        <v>180.05</v>
+        <v>119.237</v>
       </c>
       <c r="Q11" t="n">
-        <v>5.62</v>
+        <v>5.624</v>
       </c>
       <c r="R11" t="n">
-        <v>4.83</v>
+        <v>4.831</v>
       </c>
       <c r="S11" t="n">
-        <v>0.22</v>
+        <v>0.475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>